<commit_message>
Running only Suite B
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -430,7 +430,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -469,7 +469,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -502,7 +502,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3">

</xml_diff>

<commit_message>
Running only suite e
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -430,7 +430,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -469,7 +469,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -502,7 +502,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3">

</xml_diff>

<commit_message>
Running only suite F
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -430,7 +430,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -502,7 +502,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -513,7 +513,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
running profile suite only
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -480,7 +480,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -513,7 +513,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
running authoring suite only
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -430,7 +430,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -480,7 +480,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -491,7 +491,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3">

</xml_diff>

<commit_message>
Running only IAM module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>TSID</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -466,7 +469,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -477,7 +480,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -488,7 +491,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -499,7 +502,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -510,7 +513,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
running watchlist stream only
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -430,7 +430,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -458,7 +458,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -502,7 +502,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3">

</xml_diff>

<commit_message>
running C suite only
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -480,7 +480,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -491,7 +491,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3">

</xml_diff>

<commit_message>
Running E and F Suites
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -430,7 +430,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -491,7 +491,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -502,7 +502,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -513,7 +513,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Run ning suite a
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -430,7 +430,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -458,7 +458,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -469,7 +469,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3">

</xml_diff>

<commit_message>
running C and D suite only
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -430,7 +430,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -458,7 +458,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -480,7 +480,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -491,7 +491,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3">

</xml_diff>

<commit_message>
running suite D test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -430,7 +430,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -491,7 +491,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3">

</xml_diff>

<commit_message>
Checking in Suite.xlsx file
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13575" windowHeight="3690"/>
   </bookViews>
   <sheets>
     <sheet name="Test Suite" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>TSID</t>
   </si>
@@ -64,9 +65,6 @@
   </si>
   <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -430,7 +428,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -469,7 +467,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -480,7 +478,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -491,7 +489,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -502,7 +500,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -513,7 +511,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Running suites A and B parallely
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>TSID</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -477,7 +480,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -488,7 +491,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -499,7 +502,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -510,7 +513,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Running all modules except watchlist
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>TSID</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -427,7 +430,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -499,7 +502,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3">

</xml_diff>

<commit_message>
Running only watchlist module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -430,7 +430,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -458,7 +458,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -469,7 +469,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -480,7 +480,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -491,7 +491,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -502,7 +502,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -513,7 +513,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Running only authoring suite in Parallel.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>TSID</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -427,7 +430,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -455,7 +458,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -466,7 +469,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -488,7 +491,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -499,7 +502,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -510,7 +513,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committing code changes in suite A and suite F
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>TSID</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -427,7 +430,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -455,7 +458,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -466,7 +469,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -488,7 +491,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -499,7 +502,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -510,7 +513,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committing changes to suite E
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>TSID</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -430,7 +427,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -458,7 +455,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -469,7 +466,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -491,7 +488,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -502,7 +499,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -513,7 +510,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Running IAM test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>TSID</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -427,7 +430,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -466,7 +469,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -477,7 +480,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -488,7 +491,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -499,7 +502,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -510,7 +513,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Running only 4 modules
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -430,7 +430,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -458,7 +458,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -469,7 +469,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -491,7 +491,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -502,7 +502,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -513,7 +513,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committing the changes for proper extent report
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>TSID</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -430,7 +427,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -458,7 +455,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -469,7 +466,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -491,7 +488,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -502,7 +499,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -513,7 +510,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed Notifications module Run mode = N
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>TSID</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -427,7 +430,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -510,7 +513,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changing run mode in Suite.xlsx
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13575" windowHeight="3690"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="12150" windowHeight="4020"/>
   </bookViews>
   <sheets>
     <sheet name="Test Suite" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>TSID</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -430,7 +427,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C2" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -513,7 +510,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Framework Changes made to IAM module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -30,9 +30,6 @@
     <t>B Suite</t>
   </si>
   <si>
-    <t>A Suite</t>
-  </si>
-  <si>
     <t>IAM module</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>IAM</t>
   </si>
 </sst>
 </file>
@@ -427,7 +427,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -449,13 +449,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -463,54 +463,54 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modifying variable name from suiteDxls to watchlistXls
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>TSID</t>
   </si>
@@ -30,9 +30,6 @@
     <t>B Suite</t>
   </si>
   <si>
-    <t>A Suite</t>
-  </si>
-  <si>
     <t>IAM module</t>
   </si>
   <si>
@@ -63,10 +60,10 @@
     <t>Y</t>
   </si>
   <si>
+    <t>IAM</t>
+  </si>
+  <si>
     <t>Watchlist</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -430,7 +427,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C2" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -452,13 +449,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -466,32 +463,32 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -499,21 +496,21 @@
         <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding java docs to watch list scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -28,9 +28,6 @@
     <t>Runmode</t>
   </si>
   <si>
-    <t>B Suite</t>
-  </si>
-  <si>
     <t>IAM module</t>
   </si>
   <si>
@@ -65,13 +62,16 @@
   </si>
   <si>
     <t>Watchlist</t>
+  </si>
+  <si>
+    <t>Search</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,13 +79,314 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -94,12 +395,119 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -118,25 +526,101 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -428,7 +912,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -450,68 +934,68 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>6</v>
+      <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the suite name to module name.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -43,12 +42,6 @@
     <t>Notification module</t>
   </si>
   <si>
-    <t>C Suite</t>
-  </si>
-  <si>
-    <t>D Suite</t>
-  </si>
-  <si>
     <t>Authoring module</t>
   </si>
   <si>
@@ -65,6 +58,12 @@
   </si>
   <si>
     <t>Search</t>
+  </si>
+  <si>
+    <t>Authoring</t>
+  </si>
+  <si>
+    <t>Profile</t>
   </si>
 </sst>
 </file>
@@ -912,7 +911,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -934,57 +933,57 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -995,7 +994,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commiting Notification module changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -36,9 +36,6 @@
     <t>Watchlist module</t>
   </si>
   <si>
-    <t>F Suite</t>
-  </si>
-  <si>
     <t>Notification module</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
   </si>
   <si>
     <t>Profile</t>
+  </si>
+  <si>
+    <t>Notifications</t>
   </si>
 </sst>
 </file>
@@ -911,7 +911,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -933,68 +933,68 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Profile sanity testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -36,9 +36,6 @@
     <t>Watchlist module</t>
   </si>
   <si>
-    <t>F Suite</t>
-  </si>
-  <si>
     <t>Notification module</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
   </si>
   <si>
     <t>Profile</t>
+  </si>
+  <si>
+    <t>Notifications</t>
   </si>
 </sst>
 </file>
@@ -911,7 +911,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -933,68 +933,68 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removing new user dependency from watch list test scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -37,18 +36,9 @@
     <t>Watchlist module</t>
   </si>
   <si>
-    <t>F Suite</t>
-  </si>
-  <si>
     <t>Notification module</t>
   </si>
   <si>
-    <t>C Suite</t>
-  </si>
-  <si>
-    <t>D Suite</t>
-  </si>
-  <si>
     <t>Authoring module</t>
   </si>
   <si>
@@ -65,6 +55,15 @@
   </si>
   <si>
     <t>Search</t>
+  </si>
+  <si>
+    <t>Authoring</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>Notifications</t>
   </si>
 </sst>
 </file>
@@ -912,7 +911,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -934,68 +933,68 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the excel files
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>TSID</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>Notifications</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -942,7 +939,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -964,7 +961,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -975,7 +972,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -986,7 +983,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -997,7 +994,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added logs in TestBase.java
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>TSID</t>
   </si>
@@ -45,25 +45,31 @@
     <t>Profile module</t>
   </si>
   <si>
+    <t>IAM</t>
+  </si>
+  <si>
+    <t>Watchlist</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Authoring</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>Notifications</t>
+  </si>
+  <si>
     <t>Y</t>
   </si>
   <si>
-    <t>IAM</t>
-  </si>
-  <si>
-    <t>Watchlist</t>
-  </si>
-  <si>
-    <t>Search</t>
-  </si>
-  <si>
-    <t>Authoring</t>
-  </si>
-  <si>
-    <t>Profile</t>
-  </si>
-  <si>
-    <t>Notifications</t>
+    <t>Sanity suite</t>
+  </si>
+  <si>
+    <t>Sanity tests</t>
   </si>
 </sst>
 </file>
@@ -569,10 +575,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -908,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -933,68 +940,79 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
code changes are done as per removing api, ENW and LI scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>TSID</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>ENW IAM tests</t>
+  </si>
+  <si>
+    <t>LocalRun</t>
+  </si>
+  <si>
+    <t>Running only API integration,ENW and LI scripts</t>
   </si>
 </sst>
 </file>
@@ -412,7 +418,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -542,17 +548,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -598,12 +593,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -942,7 +936,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1062,7 +1056,15 @@
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="4"/>
+      <c r="A11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
IPA module is created and testcaes are added
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2580" windowWidth="10305" windowHeight="3150"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>TSID</t>
   </si>
@@ -94,13 +94,19 @@
   </si>
   <si>
     <t>DRA test cases</t>
+  </si>
+  <si>
+    <t>IPA</t>
+  </si>
+  <si>
+    <t>IPA test cases</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -734,7 +740,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -769,7 +774,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -945,20 +949,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:C12"/>
+      <selection activeCell="A13" sqref="A13:C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -969,7 +973,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -980,7 +984,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -991,7 +995,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -1002,7 +1006,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -1013,7 +1017,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1024,7 +1028,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -1035,7 +1039,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -1046,7 +1050,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
@@ -1057,7 +1061,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
@@ -1068,7 +1072,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
@@ -1079,7 +1083,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
@@ -1087,6 +1091,17 @@
         <v>25</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1097,24 +1112,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
renamed dra to draiam suite
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -90,9 +90,6 @@
     <t>Running only API integration,ENW and LI scripts</t>
   </si>
   <si>
-    <t>DRA</t>
-  </si>
-  <si>
     <t>DRA test cases</t>
   </si>
   <si>
@@ -106,6 +103,9 @@
   </si>
   <si>
     <t>IPA IAM test casess</t>
+  </si>
+  <si>
+    <t>DRAIAM</t>
   </si>
 </sst>
 </file>
@@ -976,7 +976,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,10 +1108,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>15</v>
@@ -1119,10 +1119,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>15</v>
@@ -1130,10 +1130,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
WAT application Automation scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16005" windowHeight="5985"/>
@@ -11,13 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
   <si>
     <t>TSID</t>
   </si>
@@ -119,13 +118,19 @@
   </si>
   <si>
     <t>customercare Module test cases</t>
+  </si>
+  <si>
+    <t>WAT</t>
+  </si>
+  <si>
+    <t>WoS Author Transformation testcases</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -730,7 +735,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -762,10 +767,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -797,7 +801,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -973,20 +976,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -997,7 +1000,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -1008,7 +1011,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -1019,7 +1022,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -1030,7 +1033,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -1041,7 +1044,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1052,7 +1055,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -1063,7 +1066,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -1074,7 +1077,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
@@ -1085,7 +1088,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
@@ -1096,7 +1099,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
@@ -1107,7 +1110,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
@@ -1118,7 +1121,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="3" t="s">
         <v>25</v>
       </c>
@@ -1129,7 +1132,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
@@ -1140,7 +1143,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
@@ -1151,7 +1154,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" s="3" t="s">
         <v>32</v>
       </c>
@@ -1159,6 +1162,17 @@
         <v>33</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1169,24 +1183,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Created new publons module in ui automation framework
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15576" windowHeight="5988"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15570" windowHeight="5985"/>
   </bookViews>
   <sheets>
     <sheet name="Test Suite" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
   <si>
     <t>TSID</t>
   </si>
@@ -130,13 +130,19 @@
   </si>
   <si>
     <t>WoS Author Transformation IAM testcases</t>
+  </si>
+  <si>
+    <t>PUBLONS</t>
+  </si>
+  <si>
+    <t>PUBLONS module</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -741,7 +747,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -773,9 +779,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -807,6 +814,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -982,20 +990,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1006,7 +1014,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -1017,7 +1025,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -1028,7 +1036,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -1039,7 +1047,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -1050,7 +1058,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1061,7 +1069,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -1072,7 +1080,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -1083,7 +1091,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
@@ -1094,7 +1102,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
@@ -1105,7 +1113,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
@@ -1116,7 +1124,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
@@ -1127,7 +1135,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>25</v>
       </c>
@@ -1138,7 +1146,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
@@ -1149,7 +1157,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
@@ -1160,7 +1168,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>32</v>
       </c>
@@ -1171,7 +1179,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>34</v>
       </c>
@@ -1182,7 +1190,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>36</v>
       </c>
@@ -1190,6 +1198,17 @@
         <v>37</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1200,24 +1219,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
code refactoring has been done for WAT/RRC project
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Suite.xlsx
+++ b/src/test/resources/xls/Suite.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15570" windowHeight="5985"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>TSID</t>
   </si>
@@ -27,97 +27,7 @@
     <t>Runmode</t>
   </si>
   <si>
-    <t>IAM module</t>
-  </si>
-  <si>
-    <t>Search module</t>
-  </si>
-  <si>
-    <t>Watchlist module</t>
-  </si>
-  <si>
-    <t>Notification module</t>
-  </si>
-  <si>
-    <t>Authoring module</t>
-  </si>
-  <si>
-    <t>Profile module</t>
-  </si>
-  <si>
-    <t>IAM</t>
-  </si>
-  <si>
-    <t>Watchlist</t>
-  </si>
-  <si>
-    <t>Search</t>
-  </si>
-  <si>
-    <t>Authoring</t>
-  </si>
-  <si>
-    <t>Profile</t>
-  </si>
-  <si>
-    <t>Notifications</t>
-  </si>
-  <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>Sanity suite</t>
-  </si>
-  <si>
-    <t>Sanity tests</t>
-  </si>
-  <si>
-    <t>ENW</t>
-  </si>
-  <si>
-    <t>ENW tests</t>
-  </si>
-  <si>
-    <t>ENWIAM</t>
-  </si>
-  <si>
-    <t>ENW IAM tests</t>
-  </si>
-  <si>
-    <t>LocalRun</t>
-  </si>
-  <si>
-    <t>Running only API integration,ENW and LI scripts</t>
-  </si>
-  <si>
-    <t>DRA test cases</t>
-  </si>
-  <si>
-    <t>IPA</t>
-  </si>
-  <si>
-    <t>IPA test cases</t>
-  </si>
-  <si>
-    <t>IPAIAM</t>
-  </si>
-  <si>
-    <t>DRAIAM</t>
-  </si>
-  <si>
-    <t>RCC</t>
-  </si>
-  <si>
-    <t>IPA IAM test cases</t>
-  </si>
-  <si>
-    <t>RCC Module test cases</t>
-  </si>
-  <si>
-    <t>customercare</t>
-  </si>
-  <si>
-    <t>customercare Module test cases</t>
   </si>
   <si>
     <t>WAT</t>
@@ -131,18 +41,12 @@
   <si>
     <t>WoS Author Transformation IAM testcases</t>
   </si>
-  <si>
-    <t>PUBLONS</t>
-  </si>
-  <si>
-    <t>PUBLONS module</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -641,10 +545,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -747,7 +650,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -779,10 +682,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -814,7 +716,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -990,20 +891,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1014,202 +915,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1219,24 +944,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>